<commit_message>
20211224 delete initial Population
</commit_message>
<xml_diff>
--- a/Excel/test.xlsx
+++ b/Excel/test.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="TSP" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="test.xlsx" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,10 +458,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1041530589573085</v>
+        <v>0.09198384601040743</v>
       </c>
       <c r="D2" t="n">
-        <v>605</v>
+        <v>633</v>
       </c>
     </row>
     <row r="3">
@@ -472,10 +472,1382 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1789227349217981</v>
+        <v>0.1781212520145345</v>
       </c>
       <c r="D3" t="n">
-        <v>605</v>
+        <v>597</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="n">
+        <v>3</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.269107736996375</v>
+      </c>
+      <c r="D4" t="n">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.342146003007656</v>
+      </c>
+      <c r="D5" t="n">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.4206069369975012</v>
+      </c>
+      <c r="D6" t="n">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="n">
+        <v>6</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.5006895779806655</v>
+      </c>
+      <c r="D7" t="n">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.586960904969601</v>
+      </c>
+      <c r="D8" t="n">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.6541185189562384</v>
+      </c>
+      <c r="D9" t="n">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.7372124609537423</v>
+      </c>
+      <c r="D10" t="n">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.8328580279776361</v>
+      </c>
+      <c r="D11" t="n">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.9062016709940508</v>
+      </c>
+      <c r="D12" t="n">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.9999750179995317</v>
+      </c>
+      <c r="D13" t="n">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="n">
+        <v>13</v>
+      </c>
+      <c r="C14" t="n">
+        <v>1.091117081989069</v>
+      </c>
+      <c r="D14" t="n">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="n">
+        <v>14</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1.191667078965111</v>
+      </c>
+      <c r="D15" t="n">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="n">
+        <v>15</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1.275243157957448</v>
+      </c>
+      <c r="D16" t="n">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="n">
+        <v>16</v>
+      </c>
+      <c r="C17" t="n">
+        <v>1.342634590953821</v>
+      </c>
+      <c r="D17" t="n">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="n">
+        <v>17</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1.427363576949574</v>
+      </c>
+      <c r="D18" t="n">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="n">
+        <v>18</v>
+      </c>
+      <c r="C19" t="n">
+        <v>1.496437236957718</v>
+      </c>
+      <c r="D19" t="n">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="n">
+        <v>19</v>
+      </c>
+      <c r="C20" t="n">
+        <v>1.580496748967562</v>
+      </c>
+      <c r="D20" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="n">
+        <v>20</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1.661938875971828</v>
+      </c>
+      <c r="D21" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="n">
+        <v>21</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1.743820915988181</v>
+      </c>
+      <c r="D22" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="n">
+        <v>22</v>
+      </c>
+      <c r="C23" t="n">
+        <v>1.823040057963226</v>
+      </c>
+      <c r="D23" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>23</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1.912801483966177</v>
+      </c>
+      <c r="D24" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="n">
+        <v>24</v>
+      </c>
+      <c r="C25" t="n">
+        <v>2.009831337985815</v>
+      </c>
+      <c r="D25" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="n">
+        <v>25</v>
+      </c>
+      <c r="C26" t="n">
+        <v>2.09983251299127</v>
+      </c>
+      <c r="D26" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="n">
+        <v>26</v>
+      </c>
+      <c r="C27" t="n">
+        <v>2.184130865993211</v>
+      </c>
+      <c r="D27" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="n">
+        <v>27</v>
+      </c>
+      <c r="C28" t="n">
+        <v>2.269432667992078</v>
+      </c>
+      <c r="D28" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="n">
+        <v>28</v>
+      </c>
+      <c r="C29" t="n">
+        <v>2.357159844978014</v>
+      </c>
+      <c r="D29" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="n">
+        <v>29</v>
+      </c>
+      <c r="C30" t="n">
+        <v>2.445518657972571</v>
+      </c>
+      <c r="D30" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="n">
+        <v>30</v>
+      </c>
+      <c r="C31" t="n">
+        <v>2.52181456895778</v>
+      </c>
+      <c r="D31" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="n">
+        <v>31</v>
+      </c>
+      <c r="C32" t="n">
+        <v>2.608006585971452</v>
+      </c>
+      <c r="D32" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="n">
+        <v>32</v>
+      </c>
+      <c r="C33" t="n">
+        <v>2.688508443970932</v>
+      </c>
+      <c r="D33" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="n">
+        <v>33</v>
+      </c>
+      <c r="C34" t="n">
+        <v>2.762988819973543</v>
+      </c>
+      <c r="D34" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="n">
+        <v>34</v>
+      </c>
+      <c r="C35" t="n">
+        <v>2.84368864595308</v>
+      </c>
+      <c r="D35" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="n">
+        <v>35</v>
+      </c>
+      <c r="C36" t="n">
+        <v>2.934952143958071</v>
+      </c>
+      <c r="D36" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="n">
+        <v>36</v>
+      </c>
+      <c r="C37" t="n">
+        <v>3.01556917396374</v>
+      </c>
+      <c r="D37" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="n">
+        <v>37</v>
+      </c>
+      <c r="C38" t="n">
+        <v>3.088028480968205</v>
+      </c>
+      <c r="D38" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="n">
+        <v>38</v>
+      </c>
+      <c r="C39" t="n">
+        <v>3.172797890962102</v>
+      </c>
+      <c r="D39" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="n">
+        <v>39</v>
+      </c>
+      <c r="C40" t="n">
+        <v>3.264319860958494</v>
+      </c>
+      <c r="D40" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="n">
+        <v>40</v>
+      </c>
+      <c r="C41" t="n">
+        <v>3.362091332965065</v>
+      </c>
+      <c r="D41" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="n">
+        <v>41</v>
+      </c>
+      <c r="C42" t="n">
+        <v>3.451814115978777</v>
+      </c>
+      <c r="D42" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="n">
+        <v>42</v>
+      </c>
+      <c r="C43" t="n">
+        <v>3.526491044962313</v>
+      </c>
+      <c r="D43" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="n">
+        <v>43</v>
+      </c>
+      <c r="C44" t="n">
+        <v>3.613344792946009</v>
+      </c>
+      <c r="D44" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="n">
+        <v>44</v>
+      </c>
+      <c r="C45" t="n">
+        <v>3.705892654950731</v>
+      </c>
+      <c r="D45" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="n">
+        <v>45</v>
+      </c>
+      <c r="C46" t="n">
+        <v>3.779418520949548</v>
+      </c>
+      <c r="D46" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="n">
+        <v>46</v>
+      </c>
+      <c r="C47" t="n">
+        <v>3.871915797964903</v>
+      </c>
+      <c r="D47" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="n">
+        <v>47</v>
+      </c>
+      <c r="C48" t="n">
+        <v>3.948349207959836</v>
+      </c>
+      <c r="D48" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="1" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="n">
+        <v>48</v>
+      </c>
+      <c r="C49" t="n">
+        <v>4.040541424968978</v>
+      </c>
+      <c r="D49" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="1" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="n">
+        <v>49</v>
+      </c>
+      <c r="C50" t="n">
+        <v>4.140698435949162</v>
+      </c>
+      <c r="D50" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="1" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="n">
+        <v>50</v>
+      </c>
+      <c r="C51" t="n">
+        <v>4.231796529929852</v>
+      </c>
+      <c r="D51" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="1" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="n">
+        <v>51</v>
+      </c>
+      <c r="C52" t="n">
+        <v>4.301828809926519</v>
+      </c>
+      <c r="D52" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="n">
+        <v>52</v>
+      </c>
+      <c r="C53" t="n">
+        <v>4.380436361941975</v>
+      </c>
+      <c r="D53" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="1" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="n">
+        <v>53</v>
+      </c>
+      <c r="C54" t="n">
+        <v>4.474200901953736</v>
+      </c>
+      <c r="D54" t="n">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="1" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="n">
+        <v>54</v>
+      </c>
+      <c r="C55" t="n">
+        <v>4.542840431939112</v>
+      </c>
+      <c r="D55" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="1" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="n">
+        <v>55</v>
+      </c>
+      <c r="C56" t="n">
+        <v>4.62071023194585</v>
+      </c>
+      <c r="D56" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="n">
+        <v>56</v>
+      </c>
+      <c r="C57" t="n">
+        <v>4.711861606949242</v>
+      </c>
+      <c r="D57" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="1" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="n">
+        <v>57</v>
+      </c>
+      <c r="C58" t="n">
+        <v>4.784773696941556</v>
+      </c>
+      <c r="D58" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="1" t="n">
+        <v>57</v>
+      </c>
+      <c r="B59" t="n">
+        <v>58</v>
+      </c>
+      <c r="C59" t="n">
+        <v>4.875607793946983</v>
+      </c>
+      <c r="D59" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="1" t="n">
+        <v>58</v>
+      </c>
+      <c r="B60" t="n">
+        <v>59</v>
+      </c>
+      <c r="C60" t="n">
+        <v>4.966864262969466</v>
+      </c>
+      <c r="D60" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="1" t="n">
+        <v>59</v>
+      </c>
+      <c r="B61" t="n">
+        <v>60</v>
+      </c>
+      <c r="C61" t="n">
+        <v>5.052465879969532</v>
+      </c>
+      <c r="D61" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="1" t="n">
+        <v>60</v>
+      </c>
+      <c r="B62" t="n">
+        <v>61</v>
+      </c>
+      <c r="C62" t="n">
+        <v>5.136684014985804</v>
+      </c>
+      <c r="D62" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B63" t="n">
+        <v>62</v>
+      </c>
+      <c r="C63" t="n">
+        <v>5.215852916997392</v>
+      </c>
+      <c r="D63" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="1" t="n">
+        <v>62</v>
+      </c>
+      <c r="B64" t="n">
+        <v>63</v>
+      </c>
+      <c r="C64" t="n">
+        <v>5.289315137983067</v>
+      </c>
+      <c r="D64" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="1" t="n">
+        <v>63</v>
+      </c>
+      <c r="B65" t="n">
+        <v>64</v>
+      </c>
+      <c r="C65" t="n">
+        <v>5.370160210004542</v>
+      </c>
+      <c r="D65" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="1" t="n">
+        <v>64</v>
+      </c>
+      <c r="B66" t="n">
+        <v>65</v>
+      </c>
+      <c r="C66" t="n">
+        <v>5.450488132017199</v>
+      </c>
+      <c r="D66" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="1" t="n">
+        <v>65</v>
+      </c>
+      <c r="B67" t="n">
+        <v>66</v>
+      </c>
+      <c r="C67" t="n">
+        <v>5.532406568003353</v>
+      </c>
+      <c r="D67" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="1" t="n">
+        <v>66</v>
+      </c>
+      <c r="B68" t="n">
+        <v>67</v>
+      </c>
+      <c r="C68" t="n">
+        <v>5.624875320994761</v>
+      </c>
+      <c r="D68" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="1" t="n">
+        <v>67</v>
+      </c>
+      <c r="B69" t="n">
+        <v>68</v>
+      </c>
+      <c r="C69" t="n">
+        <v>5.701914442004636</v>
+      </c>
+      <c r="D69" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="1" t="n">
+        <v>68</v>
+      </c>
+      <c r="B70" t="n">
+        <v>69</v>
+      </c>
+      <c r="C70" t="n">
+        <v>5.77809293201426</v>
+      </c>
+      <c r="D70" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="1" t="n">
+        <v>69</v>
+      </c>
+      <c r="B71" t="n">
+        <v>70</v>
+      </c>
+      <c r="C71" t="n">
+        <v>5.8620372209989</v>
+      </c>
+      <c r="D71" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="1" t="n">
+        <v>70</v>
+      </c>
+      <c r="B72" t="n">
+        <v>71</v>
+      </c>
+      <c r="C72" t="n">
+        <v>5.9457195730065</v>
+      </c>
+      <c r="D72" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="1" t="n">
+        <v>71</v>
+      </c>
+      <c r="B73" t="n">
+        <v>72</v>
+      </c>
+      <c r="C73" t="n">
+        <v>6.029135115008103</v>
+      </c>
+      <c r="D73" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="1" t="n">
+        <v>72</v>
+      </c>
+      <c r="B74" t="n">
+        <v>73</v>
+      </c>
+      <c r="C74" t="n">
+        <v>6.110064262000378</v>
+      </c>
+      <c r="D74" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="1" t="n">
+        <v>73</v>
+      </c>
+      <c r="B75" t="n">
+        <v>74</v>
+      </c>
+      <c r="C75" t="n">
+        <v>6.19617732099141</v>
+      </c>
+      <c r="D75" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="1" t="n">
+        <v>74</v>
+      </c>
+      <c r="B76" t="n">
+        <v>75</v>
+      </c>
+      <c r="C76" t="n">
+        <v>6.286108414002229</v>
+      </c>
+      <c r="D76" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" s="1" t="n">
+        <v>75</v>
+      </c>
+      <c r="B77" t="n">
+        <v>76</v>
+      </c>
+      <c r="C77" t="n">
+        <v>6.387410953990184</v>
+      </c>
+      <c r="D77" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" s="1" t="n">
+        <v>76</v>
+      </c>
+      <c r="B78" t="n">
+        <v>77</v>
+      </c>
+      <c r="C78" t="n">
+        <v>6.470975105010439</v>
+      </c>
+      <c r="D78" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" s="1" t="n">
+        <v>77</v>
+      </c>
+      <c r="B79" t="n">
+        <v>78</v>
+      </c>
+      <c r="C79" t="n">
+        <v>6.544915968028363</v>
+      </c>
+      <c r="D79" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" s="1" t="n">
+        <v>78</v>
+      </c>
+      <c r="B80" t="n">
+        <v>79</v>
+      </c>
+      <c r="C80" t="n">
+        <v>6.62984417102416</v>
+      </c>
+      <c r="D80" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="1" t="n">
+        <v>79</v>
+      </c>
+      <c r="B81" t="n">
+        <v>80</v>
+      </c>
+      <c r="C81" t="n">
+        <v>6.692090813041432</v>
+      </c>
+      <c r="D81" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" s="1" t="n">
+        <v>80</v>
+      </c>
+      <c r="B82" t="n">
+        <v>81</v>
+      </c>
+      <c r="C82" t="n">
+        <v>6.786676468036603</v>
+      </c>
+      <c r="D82" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" s="1" t="n">
+        <v>81</v>
+      </c>
+      <c r="B83" t="n">
+        <v>82</v>
+      </c>
+      <c r="C83" t="n">
+        <v>6.884075431036763</v>
+      </c>
+      <c r="D83" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" s="1" t="n">
+        <v>82</v>
+      </c>
+      <c r="B84" t="n">
+        <v>83</v>
+      </c>
+      <c r="C84" t="n">
+        <v>6.973719999048626</v>
+      </c>
+      <c r="D84" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" s="1" t="n">
+        <v>83</v>
+      </c>
+      <c r="B85" t="n">
+        <v>84</v>
+      </c>
+      <c r="C85" t="n">
+        <v>7.053396033064928</v>
+      </c>
+      <c r="D85" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" s="1" t="n">
+        <v>84</v>
+      </c>
+      <c r="B86" t="n">
+        <v>85</v>
+      </c>
+      <c r="C86" t="n">
+        <v>7.126371971069602</v>
+      </c>
+      <c r="D86" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B87" t="n">
+        <v>86</v>
+      </c>
+      <c r="C87" t="n">
+        <v>7.213120450061979</v>
+      </c>
+      <c r="D87" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" s="1" t="n">
+        <v>86</v>
+      </c>
+      <c r="B88" t="n">
+        <v>87</v>
+      </c>
+      <c r="C88" t="n">
+        <v>7.299240324064158</v>
+      </c>
+      <c r="D88" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" s="1" t="n">
+        <v>87</v>
+      </c>
+      <c r="B89" t="n">
+        <v>88</v>
+      </c>
+      <c r="C89" t="n">
+        <v>7.374306439072825</v>
+      </c>
+      <c r="D89" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" s="1" t="n">
+        <v>88</v>
+      </c>
+      <c r="B90" t="n">
+        <v>89</v>
+      </c>
+      <c r="C90" t="n">
+        <v>7.462247438088525</v>
+      </c>
+      <c r="D90" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" s="1" t="n">
+        <v>89</v>
+      </c>
+      <c r="B91" t="n">
+        <v>90</v>
+      </c>
+      <c r="C91" t="n">
+        <v>7.562772425095318</v>
+      </c>
+      <c r="D91" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" s="1" t="n">
+        <v>90</v>
+      </c>
+      <c r="B92" t="n">
+        <v>91</v>
+      </c>
+      <c r="C92" t="n">
+        <v>7.667573112092214</v>
+      </c>
+      <c r="D92" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" s="1" t="n">
+        <v>91</v>
+      </c>
+      <c r="B93" t="n">
+        <v>92</v>
+      </c>
+      <c r="C93" t="n">
+        <v>7.736926447105361</v>
+      </c>
+      <c r="D93" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" s="1" t="n">
+        <v>92</v>
+      </c>
+      <c r="B94" t="n">
+        <v>93</v>
+      </c>
+      <c r="C94" t="n">
+        <v>7.817557116097305</v>
+      </c>
+      <c r="D94" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" s="1" t="n">
+        <v>93</v>
+      </c>
+      <c r="B95" t="n">
+        <v>94</v>
+      </c>
+      <c r="C95" t="n">
+        <v>7.915646050096257</v>
+      </c>
+      <c r="D95" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" s="1" t="n">
+        <v>94</v>
+      </c>
+      <c r="B96" t="n">
+        <v>95</v>
+      </c>
+      <c r="C96" t="n">
+        <v>8.010158317076275</v>
+      </c>
+      <c r="D96" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" s="1" t="n">
+        <v>95</v>
+      </c>
+      <c r="B97" t="n">
+        <v>96</v>
+      </c>
+      <c r="C97" t="n">
+        <v>8.088924083072925</v>
+      </c>
+      <c r="D97" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="B98" t="n">
+        <v>97</v>
+      </c>
+      <c r="C98" t="n">
+        <v>8.176564083085395</v>
+      </c>
+      <c r="D98" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="1" t="n">
+        <v>97</v>
+      </c>
+      <c r="B99" t="n">
+        <v>98</v>
+      </c>
+      <c r="C99" t="n">
+        <v>8.262515522073954</v>
+      </c>
+      <c r="D99" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="1" t="n">
+        <v>98</v>
+      </c>
+      <c r="B100" t="n">
+        <v>99</v>
+      </c>
+      <c r="C100" t="n">
+        <v>8.342265581071842</v>
+      </c>
+      <c r="D100" t="n">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="1" t="n">
+        <v>99</v>
+      </c>
+      <c r="B101" t="n">
+        <v>100</v>
+      </c>
+      <c r="C101" t="n">
+        <v>8.442027491051704</v>
+      </c>
+      <c r="D101" t="n">
+        <v>585</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20210103 For experiment enhancement
</commit_message>
<xml_diff>
--- a/Excel/test.xlsx
+++ b/Excel/test.xlsx
@@ -458,10 +458,10 @@
         <v>1</v>
       </c>
       <c r="C2" t="n">
-        <v>0.1687879999954021</v>
+        <v>0.2588880590010376</v>
       </c>
       <c r="D2" t="n">
-        <v>616</v>
+        <v>592</v>
       </c>
     </row>
     <row r="3">
@@ -472,10 +472,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="n">
-        <v>0.3988611949898768</v>
+        <v>0.5035661390002133</v>
       </c>
       <c r="D3" t="n">
-        <v>610</v>
+        <v>592</v>
       </c>
     </row>
     <row r="4">
@@ -486,10 +486,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="n">
-        <v>0.6324213869811501</v>
+        <v>0.7889680520002003</v>
       </c>
       <c r="D4" t="n">
-        <v>598</v>
+        <v>582</v>
       </c>
     </row>
     <row r="5">
@@ -500,10 +500,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="n">
-        <v>0.8668908579857089</v>
+        <v>0.9818535060003342</v>
       </c>
       <c r="D5" t="n">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="6">
@@ -514,10 +514,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="n">
-        <v>1.05763206697884</v>
+        <v>1.216101214999981</v>
       </c>
       <c r="D6" t="n">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="7">
@@ -528,10 +528,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="n">
-        <v>1.264221915975213</v>
+        <v>1.484270068000114</v>
       </c>
       <c r="D7" t="n">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="8">
@@ -542,10 +542,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="n">
-        <v>1.510984217980877</v>
+        <v>1.755511155000022</v>
       </c>
       <c r="D8" t="n">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="9">
@@ -556,7 +556,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="n">
-        <v>1.776149908982916</v>
+        <v>2.107468427999265</v>
       </c>
       <c r="D9" t="n">
         <v>581</v>
@@ -570,7 +570,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>1.994328715984011</v>
+        <v>2.377706694998778</v>
       </c>
       <c r="D10" t="n">
         <v>581</v>
@@ -584,7 +584,7 @@
         <v>10</v>
       </c>
       <c r="C11" t="n">
-        <v>2.248113839988946</v>
+        <v>2.642980797998462</v>
       </c>
       <c r="D11" t="n">
         <v>581</v>
@@ -598,7 +598,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="n">
-        <v>2.525818412992521</v>
+        <v>2.94413090299895</v>
       </c>
       <c r="D12" t="n">
         <v>581</v>
@@ -612,7 +612,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="n">
-        <v>2.717848530985066</v>
+        <v>3.257306075999622</v>
       </c>
       <c r="D13" t="n">
         <v>581</v>
@@ -626,7 +626,7 @@
         <v>13</v>
       </c>
       <c r="C14" t="n">
-        <v>2.911195063978084</v>
+        <v>3.552105666999523</v>
       </c>
       <c r="D14" t="n">
         <v>581</v>
@@ -640,10 +640,10 @@
         <v>14</v>
       </c>
       <c r="C15" t="n">
-        <v>3.129616988982889</v>
+        <v>3.827662147999945</v>
       </c>
       <c r="D15" t="n">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="16">
@@ -654,10 +654,10 @@
         <v>15</v>
       </c>
       <c r="C16" t="n">
-        <v>3.335643164988142</v>
+        <v>4.15952117300003</v>
       </c>
       <c r="D16" t="n">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="17">
@@ -668,10 +668,10 @@
         <v>16</v>
       </c>
       <c r="C17" t="n">
-        <v>3.566367974985042</v>
+        <v>4.467262455000309</v>
       </c>
       <c r="D17" t="n">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="18">
@@ -682,10 +682,10 @@
         <v>17</v>
       </c>
       <c r="C18" t="n">
-        <v>3.7852903399762</v>
+        <v>4.642935534000571</v>
       </c>
       <c r="D18" t="n">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="19">
@@ -696,10 +696,10 @@
         <v>18</v>
       </c>
       <c r="C19" t="n">
-        <v>3.976121889980277</v>
+        <v>4.866894922000029</v>
       </c>
       <c r="D19" t="n">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="20">
@@ -710,10 +710,10 @@
         <v>19</v>
       </c>
       <c r="C20" t="n">
-        <v>4.235213347972604</v>
+        <v>5.156737407000037</v>
       </c>
       <c r="D20" t="n">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="21">
@@ -724,10 +724,10 @@
         <v>20</v>
       </c>
       <c r="C21" t="n">
-        <v>4.451499590970343</v>
+        <v>5.378081793999627</v>
       </c>
       <c r="D21" t="n">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="22">
@@ -738,10 +738,10 @@
         <v>21</v>
       </c>
       <c r="C22" t="n">
-        <v>4.759383829979924</v>
+        <v>5.645050753999385</v>
       </c>
       <c r="D22" t="n">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="23">
@@ -752,10 +752,10 @@
         <v>22</v>
       </c>
       <c r="C23" t="n">
-        <v>4.92979560297681</v>
+        <v>5.871087968998836</v>
       </c>
       <c r="D23" t="n">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="24">
@@ -766,10 +766,10 @@
         <v>23</v>
       </c>
       <c r="C24" t="n">
-        <v>5.121534964971943</v>
+        <v>6.040054819998659</v>
       </c>
       <c r="D24" t="n">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="25">
@@ -780,10 +780,10 @@
         <v>24</v>
       </c>
       <c r="C25" t="n">
-        <v>5.249919935973594</v>
+        <v>6.326487558998451</v>
       </c>
       <c r="D25" t="n">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="26">
@@ -794,10 +794,10 @@
         <v>25</v>
       </c>
       <c r="C26" t="n">
-        <v>5.515629163972335</v>
+        <v>6.589295155998116</v>
       </c>
       <c r="D26" t="n">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="27">
@@ -808,10 +808,10 @@
         <v>26</v>
       </c>
       <c r="C27" t="n">
-        <v>5.722230398969259</v>
+        <v>6.855491790998713</v>
       </c>
       <c r="D27" t="n">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="28">
@@ -822,10 +822,10 @@
         <v>27</v>
       </c>
       <c r="C28" t="n">
-        <v>5.900214274966856</v>
+        <v>7.161866936998194</v>
       </c>
       <c r="D28" t="n">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="29">
@@ -836,10 +836,10 @@
         <v>28</v>
       </c>
       <c r="C29" t="n">
-        <v>6.113151740966714</v>
+        <v>7.490124142997956</v>
       </c>
       <c r="D29" t="n">
-        <v>580</v>
+        <v>581</v>
       </c>
     </row>
     <row r="30">
@@ -850,10 +850,10 @@
         <v>29</v>
       </c>
       <c r="C30" t="n">
-        <v>6.304868842969881</v>
+        <v>7.815030941997975</v>
       </c>
       <c r="D30" t="n">
-        <v>577</v>
+        <v>581</v>
       </c>
     </row>
     <row r="31">
@@ -864,10 +864,10 @@
         <v>30</v>
       </c>
       <c r="C31" t="n">
-        <v>6.564407715966809</v>
+        <v>8.031460918998164</v>
       </c>
       <c r="D31" t="n">
-        <v>577</v>
+        <v>581</v>
       </c>
     </row>
     <row r="32">
@@ -878,10 +878,10 @@
         <v>31</v>
       </c>
       <c r="C32" t="n">
-        <v>6.77573465097521</v>
+        <v>8.284992943998077</v>
       </c>
       <c r="D32" t="n">
-        <v>577</v>
+        <v>581</v>
       </c>
     </row>
     <row r="33">
@@ -892,10 +892,10 @@
         <v>32</v>
       </c>
       <c r="C33" t="n">
-        <v>6.990294081973843</v>
+        <v>8.522040217998438</v>
       </c>
       <c r="D33" t="n">
-        <v>577</v>
+        <v>581</v>
       </c>
     </row>
     <row r="34">
@@ -906,10 +906,10 @@
         <v>33</v>
       </c>
       <c r="C34" t="n">
-        <v>7.306996597981197</v>
+        <v>8.706479695998496</v>
       </c>
       <c r="D34" t="n">
-        <v>577</v>
+        <v>581</v>
       </c>
     </row>
     <row r="35">
@@ -920,10 +920,10 @@
         <v>34</v>
       </c>
       <c r="C35" t="n">
-        <v>7.521681538972189</v>
+        <v>8.986557467997955</v>
       </c>
       <c r="D35" t="n">
-        <v>577</v>
+        <v>581</v>
       </c>
     </row>
     <row r="36">
@@ -934,10 +934,10 @@
         <v>35</v>
       </c>
       <c r="C36" t="n">
-        <v>7.713419565960066</v>
+        <v>9.247064877998127</v>
       </c>
       <c r="D36" t="n">
-        <v>577</v>
+        <v>581</v>
       </c>
     </row>
     <row r="37">
@@ -948,10 +948,10 @@
         <v>36</v>
       </c>
       <c r="C37" t="n">
-        <v>7.838303080963669</v>
+        <v>9.535354276998078</v>
       </c>
       <c r="D37" t="n">
-        <v>577</v>
+        <v>581</v>
       </c>
     </row>
     <row r="38">
@@ -962,10 +962,10 @@
         <v>37</v>
       </c>
       <c r="C38" t="n">
-        <v>7.991335326965782</v>
+        <v>9.835632147997785</v>
       </c>
       <c r="D38" t="n">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="39">
@@ -976,10 +976,10 @@
         <v>38</v>
       </c>
       <c r="C39" t="n">
-        <v>8.154847438971046</v>
+        <v>10.11193685399758</v>
       </c>
       <c r="D39" t="n">
-        <v>576</v>
+        <v>579</v>
       </c>
     </row>
     <row r="40">
@@ -990,10 +990,10 @@
         <v>39</v>
       </c>
       <c r="C40" t="n">
-        <v>8.341304453962948</v>
+        <v>10.35034233999795</v>
       </c>
       <c r="D40" t="n">
-        <v>576</v>
+        <v>579</v>
       </c>
     </row>
     <row r="41">
@@ -1004,10 +1004,10 @@
         <v>40</v>
       </c>
       <c r="C41" t="n">
-        <v>8.504549211953417</v>
+        <v>10.69565068599786</v>
       </c>
       <c r="D41" t="n">
-        <v>576</v>
+        <v>579</v>
       </c>
     </row>
     <row r="42">
@@ -1018,10 +1018,10 @@
         <v>41</v>
       </c>
       <c r="C42" t="n">
-        <v>8.732810801957385</v>
+        <v>11.07080998499805</v>
       </c>
       <c r="D42" t="n">
-        <v>576</v>
+        <v>579</v>
       </c>
     </row>
     <row r="43">
@@ -1032,10 +1032,10 @@
         <v>42</v>
       </c>
       <c r="C43" t="n">
-        <v>8.930425321945222</v>
+        <v>11.34120469099798</v>
       </c>
       <c r="D43" t="n">
-        <v>576</v>
+        <v>579</v>
       </c>
     </row>
     <row r="44">
@@ -1046,10 +1046,10 @@
         <v>43</v>
       </c>
       <c r="C44" t="n">
-        <v>9.113653472944861</v>
+        <v>11.66284124999856</v>
       </c>
       <c r="D44" t="n">
-        <v>576</v>
+        <v>579</v>
       </c>
     </row>
     <row r="45">
@@ -1060,10 +1060,10 @@
         <v>44</v>
       </c>
       <c r="C45" t="n">
-        <v>9.296354093938135</v>
+        <v>11.97010518399838</v>
       </c>
       <c r="D45" t="n">
-        <v>576</v>
+        <v>579</v>
       </c>
     </row>
     <row r="46">
@@ -1074,10 +1074,10 @@
         <v>45</v>
       </c>
       <c r="C46" t="n">
-        <v>9.522675320928101</v>
+        <v>12.21920836599838</v>
       </c>
       <c r="D46" t="n">
-        <v>576</v>
+        <v>579</v>
       </c>
     </row>
     <row r="47">
@@ -1088,10 +1088,10 @@
         <v>46</v>
       </c>
       <c r="C47" t="n">
-        <v>9.810649718929199</v>
+        <v>12.50621331599905</v>
       </c>
       <c r="D47" t="n">
-        <v>576</v>
+        <v>579</v>
       </c>
     </row>
     <row r="48">
@@ -1102,10 +1102,10 @@
         <v>47</v>
       </c>
       <c r="C48" t="n">
-        <v>10.0586175169301</v>
+        <v>12.88723637799922</v>
       </c>
       <c r="D48" t="n">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="49">
@@ -1116,10 +1116,10 @@
         <v>48</v>
       </c>
       <c r="C49" t="n">
-        <v>10.27681719092652</v>
+        <v>13.09753182599889</v>
       </c>
       <c r="D49" t="n">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="50">
@@ -1130,10 +1130,10 @@
         <v>49</v>
       </c>
       <c r="C50" t="n">
-        <v>10.53153870592359</v>
+        <v>13.34658312499869</v>
       </c>
       <c r="D50" t="n">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="51">
@@ -1144,10 +1144,10 @@
         <v>50</v>
       </c>
       <c r="C51" t="n">
-        <v>10.73570023493085</v>
+        <v>13.5534428539986</v>
       </c>
       <c r="D51" t="n">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="52">
@@ -1158,10 +1158,10 @@
         <v>51</v>
       </c>
       <c r="C52" t="n">
-        <v>11.00755773994024</v>
+        <v>13.78137822199824</v>
       </c>
       <c r="D52" t="n">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="53">
@@ -1172,10 +1172,10 @@
         <v>52</v>
       </c>
       <c r="C53" t="n">
-        <v>11.24383655894781</v>
+        <v>14.04427560099793</v>
       </c>
       <c r="D53" t="n">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="54">
@@ -1186,10 +1186,10 @@
         <v>53</v>
       </c>
       <c r="C54" t="n">
-        <v>11.46799630695023</v>
+        <v>14.28526698099813</v>
       </c>
       <c r="D54" t="n">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="55">
@@ -1200,10 +1200,10 @@
         <v>54</v>
       </c>
       <c r="C55" t="n">
-        <v>11.73201085094479</v>
+        <v>14.46571142599805</v>
       </c>
       <c r="D55" t="n">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="56">
@@ -1214,10 +1214,10 @@
         <v>55</v>
       </c>
       <c r="C56" t="n">
-        <v>11.97602541594824</v>
+        <v>14.68069680399731</v>
       </c>
       <c r="D56" t="n">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="57">
@@ -1228,10 +1228,10 @@
         <v>56</v>
       </c>
       <c r="C57" t="n">
-        <v>12.21463638595014</v>
+        <v>14.90298760299811</v>
       </c>
       <c r="D57" t="n">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="58">
@@ -1242,10 +1242,10 @@
         <v>57</v>
       </c>
       <c r="C58" t="n">
-        <v>12.53037355995912</v>
+        <v>15.10509822299809</v>
       </c>
       <c r="D58" t="n">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="59">
@@ -1256,10 +1256,10 @@
         <v>58</v>
       </c>
       <c r="C59" t="n">
-        <v>12.7459570379724</v>
+        <v>15.31814391799799</v>
       </c>
       <c r="D59" t="n">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="60">
@@ -1270,10 +1270,10 @@
         <v>59</v>
       </c>
       <c r="C60" t="n">
-        <v>12.96896227696561</v>
+        <v>15.56520161399749</v>
       </c>
       <c r="D60" t="n">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="61">
@@ -1284,10 +1284,10 @@
         <v>60</v>
       </c>
       <c r="C61" t="n">
-        <v>13.20638986796257</v>
+        <v>15.86397360399769</v>
       </c>
       <c r="D61" t="n">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="62">
@@ -1298,10 +1298,10 @@
         <v>61</v>
       </c>
       <c r="C62" t="n">
-        <v>13.45592474896694</v>
+        <v>16.11630798899751</v>
       </c>
       <c r="D62" t="n">
-        <v>575</v>
+        <v>579</v>
       </c>
     </row>
     <row r="63">
@@ -1312,10 +1312,10 @@
         <v>62</v>
       </c>
       <c r="C63" t="n">
-        <v>13.60423171696311</v>
+        <v>16.35316122399763</v>
       </c>
       <c r="D63" t="n">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="64">
@@ -1326,10 +1326,10 @@
         <v>63</v>
       </c>
       <c r="C64" t="n">
-        <v>13.80081609696208</v>
+        <v>16.61892146399714</v>
       </c>
       <c r="D64" t="n">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="65">
@@ -1340,10 +1340,10 @@
         <v>64</v>
       </c>
       <c r="C65" t="n">
-        <v>13.94748188897211</v>
+        <v>16.96522370799721</v>
       </c>
       <c r="D65" t="n">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="66">
@@ -1354,10 +1354,10 @@
         <v>65</v>
       </c>
       <c r="C66" t="n">
-        <v>14.10720983897045</v>
+        <v>17.26415730199733</v>
       </c>
       <c r="D66" t="n">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="67">
@@ -1368,10 +1368,10 @@
         <v>66</v>
       </c>
       <c r="C67" t="n">
-        <v>14.26255060597032</v>
+        <v>17.53253749299711</v>
       </c>
       <c r="D67" t="n">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="68">
@@ -1382,10 +1382,10 @@
         <v>67</v>
       </c>
       <c r="C68" t="n">
-        <v>14.47741055297956</v>
+        <v>17.79850726099721</v>
       </c>
       <c r="D68" t="n">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="69">
@@ -1396,10 +1396,10 @@
         <v>68</v>
       </c>
       <c r="C69" t="n">
-        <v>14.64456360298209</v>
+        <v>18.06145282899797</v>
       </c>
       <c r="D69" t="n">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="70">
@@ -1410,10 +1410,10 @@
         <v>69</v>
       </c>
       <c r="C70" t="n">
-        <v>14.8525316589803</v>
+        <v>18.34682333199817</v>
       </c>
       <c r="D70" t="n">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="71">
@@ -1424,10 +1424,10 @@
         <v>70</v>
       </c>
       <c r="C71" t="n">
-        <v>15.06106433997047</v>
+        <v>18.63151195299815</v>
       </c>
       <c r="D71" t="n">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="72">
@@ -1438,10 +1438,10 @@
         <v>71</v>
       </c>
       <c r="C72" t="n">
-        <v>15.26673034096893</v>
+        <v>18.80927865399826</v>
       </c>
       <c r="D72" t="n">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="73">
@@ -1452,10 +1452,10 @@
         <v>72</v>
       </c>
       <c r="C73" t="n">
-        <v>15.50280384697544</v>
+        <v>18.97913529699872</v>
       </c>
       <c r="D73" t="n">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="74">
@@ -1466,10 +1466,10 @@
         <v>73</v>
       </c>
       <c r="C74" t="n">
-        <v>15.66720528397127</v>
+        <v>19.16493953999816</v>
       </c>
       <c r="D74" t="n">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="75">
@@ -1480,10 +1480,10 @@
         <v>74</v>
       </c>
       <c r="C75" t="n">
-        <v>15.90851070696954</v>
+        <v>19.44286205099888</v>
       </c>
       <c r="D75" t="n">
-        <v>575</v>
+        <v>577</v>
       </c>
     </row>
     <row r="76">
@@ -1494,10 +1494,10 @@
         <v>75</v>
       </c>
       <c r="C76" t="n">
-        <v>16.21763282296888</v>
+        <v>19.71336226899894</v>
       </c>
       <c r="D76" t="n">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="77">
@@ -1508,10 +1508,10 @@
         <v>76</v>
       </c>
       <c r="C77" t="n">
-        <v>16.49162102297123</v>
+        <v>19.93776371899912</v>
       </c>
       <c r="D77" t="n">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="78">
@@ -1522,10 +1522,10 @@
         <v>77</v>
       </c>
       <c r="C78" t="n">
-        <v>16.7459936679661</v>
+        <v>20.22123807099979</v>
       </c>
       <c r="D78" t="n">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="79">
@@ -1536,10 +1536,10 @@
         <v>78</v>
       </c>
       <c r="C79" t="n">
-        <v>17.02695294196019</v>
+        <v>20.50536623599965</v>
       </c>
       <c r="D79" t="n">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="80">
@@ -1550,10 +1550,10 @@
         <v>79</v>
       </c>
       <c r="C80" t="n">
-        <v>17.24982311297208</v>
+        <v>20.75574852199952</v>
       </c>
       <c r="D80" t="n">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="81">
@@ -1564,10 +1564,10 @@
         <v>80</v>
       </c>
       <c r="C81" t="n">
-        <v>17.54181177997089</v>
+        <v>20.97906127799888</v>
       </c>
       <c r="D81" t="n">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="82">
@@ -1578,10 +1578,10 @@
         <v>81</v>
       </c>
       <c r="C82" t="n">
-        <v>17.82321582797158</v>
+        <v>21.27304938499947</v>
       </c>
       <c r="D82" t="n">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="83">
@@ -1592,10 +1592,10 @@
         <v>82</v>
       </c>
       <c r="C83" t="n">
-        <v>18.05350729897327</v>
+        <v>21.5467110489999</v>
       </c>
       <c r="D83" t="n">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="84">
@@ -1606,10 +1606,10 @@
         <v>83</v>
       </c>
       <c r="C84" t="n">
-        <v>18.20896622297005</v>
+        <v>21.81063745199936</v>
       </c>
       <c r="D84" t="n">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="85">
@@ -1620,10 +1620,10 @@
         <v>84</v>
       </c>
       <c r="C85" t="n">
-        <v>18.42271235297085</v>
+        <v>22.12620315999993</v>
       </c>
       <c r="D85" t="n">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="86">
@@ -1634,10 +1634,10 @@
         <v>85</v>
       </c>
       <c r="C86" t="n">
-        <v>18.69051275396487</v>
+        <v>22.43145007000021</v>
       </c>
       <c r="D86" t="n">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="87">
@@ -1648,10 +1648,10 @@
         <v>86</v>
       </c>
       <c r="C87" t="n">
-        <v>18.88734101995942</v>
+        <v>22.69962252799996</v>
       </c>
       <c r="D87" t="n">
-        <v>575</v>
+        <v>576</v>
       </c>
     </row>
     <row r="88">
@@ -1662,10 +1662,10 @@
         <v>87</v>
       </c>
       <c r="C88" t="n">
-        <v>19.11313251896354</v>
+        <v>23.02606948799985</v>
       </c>
       <c r="D88" t="n">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="89">
@@ -1676,10 +1676,10 @@
         <v>88</v>
       </c>
       <c r="C89" t="n">
-        <v>19.25934375096404</v>
+        <v>23.33156153999971</v>
       </c>
       <c r="D89" t="n">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="90">
@@ -1690,10 +1690,10 @@
         <v>89</v>
       </c>
       <c r="C90" t="n">
-        <v>19.43477420795534</v>
+        <v>23.6409381200001</v>
       </c>
       <c r="D90" t="n">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="91">
@@ -1704,10 +1704,10 @@
         <v>90</v>
       </c>
       <c r="C91" t="n">
-        <v>19.6027808469662</v>
+        <v>24.01073550000001</v>
       </c>
       <c r="D91" t="n">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="92">
@@ -1718,10 +1718,10 @@
         <v>91</v>
       </c>
       <c r="C92" t="n">
-        <v>19.83185972896172</v>
+        <v>24.37368441099989</v>
       </c>
       <c r="D92" t="n">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="93">
@@ -1732,10 +1732,10 @@
         <v>92</v>
       </c>
       <c r="C93" t="n">
-        <v>20.08290873895749</v>
+        <v>24.59619894000025</v>
       </c>
       <c r="D93" t="n">
-        <v>574</v>
+        <v>576</v>
       </c>
     </row>
     <row r="94">
@@ -1746,7 +1746,7 @@
         <v>93</v>
       </c>
       <c r="C94" t="n">
-        <v>20.37226544995792</v>
+        <v>24.93442203300037</v>
       </c>
       <c r="D94" t="n">
         <v>574</v>
@@ -1760,7 +1760,7 @@
         <v>94</v>
       </c>
       <c r="C95" t="n">
-        <v>20.62025436497061</v>
+        <v>25.13742411600015</v>
       </c>
       <c r="D95" t="n">
         <v>574</v>
@@ -1774,7 +1774,7 @@
         <v>95</v>
       </c>
       <c r="C96" t="n">
-        <v>20.86891026997182</v>
+        <v>25.39841622800031</v>
       </c>
       <c r="D96" t="n">
         <v>574</v>
@@ -1788,7 +1788,7 @@
         <v>96</v>
       </c>
       <c r="C97" t="n">
-        <v>21.15989677996549</v>
+        <v>25.679469918</v>
       </c>
       <c r="D97" t="n">
         <v>574</v>
@@ -1802,7 +1802,7 @@
         <v>97</v>
       </c>
       <c r="C98" t="n">
-        <v>21.3808977969602</v>
+        <v>25.99392916500074</v>
       </c>
       <c r="D98" t="n">
         <v>574</v>
@@ -1816,7 +1816,7 @@
         <v>98</v>
       </c>
       <c r="C99" t="n">
-        <v>21.61430425995786</v>
+        <v>26.28218764100075</v>
       </c>
       <c r="D99" t="n">
         <v>574</v>
@@ -1830,7 +1830,7 @@
         <v>99</v>
       </c>
       <c r="C100" t="n">
-        <v>21.87035612695036</v>
+        <v>26.53933278200111</v>
       </c>
       <c r="D100" t="n">
         <v>574</v>
@@ -1844,7 +1844,7 @@
         <v>100</v>
       </c>
       <c r="C101" t="n">
-        <v>22.13199110695859</v>
+        <v>26.87106381200101</v>
       </c>
       <c r="D101" t="n">
         <v>574</v>

</xml_diff>